<commit_message>
pre or prod arguments
</commit_message>
<xml_diff>
--- a/log/Waterschapsverordening_RTR_Pre_status_20-03-2024.xlsx
+++ b/log/Waterschapsverordening_RTR_Pre_status_20-03-2024.xlsx
@@ -124,7 +124,7 @@
     <t>2.6</t>
   </si>
   <si>
-    <t>BouwwerkOnderhouden, SlopenVanEenBouwwwerkOfDeelDaarvanOfHetVerwijderenVanAsbest, BouwwerkReinigenOfConserveren</t>
+    <t>SlopenVanEenBouwwwerkOfDeelDaarvanOfHetVerwijderenVanAsbest, BouwwerkOnderhouden, BouwwerkReinigenOfConserveren</t>
   </si>
   <si>
     <t>17-01-2024 16:00:21</t>
@@ -238,7 +238,7 @@
     <t>2.13</t>
   </si>
   <si>
-    <t>GewassenSpoelen, DrinkwaterVoorVeeKlaarmaken, GietwaterKlaarmaken, FruitSorteren</t>
+    <t>GietwaterKlaarmaken, GewassenSpoelen, DrinkwaterVoorVeeKlaarmaken, FruitSorteren</t>
   </si>
   <si>
     <t>17-01-2024 15:59:56</t>
@@ -289,7 +289,7 @@
     <t>2.16</t>
   </si>
   <si>
-    <t>BedrijfVoorTelenEnKwekenVanWaterplantenOfWaterdieren, VisvijverExploiteren</t>
+    <t>VisvijverExploiteren, BedrijfVoorTelenEnKwekenVanWaterplantenOfWaterdieren</t>
   </si>
   <si>
     <t>17-01-2024 16:00:52</t>
@@ -442,7 +442,7 @@
     <t>4.7.2</t>
   </si>
   <si>
-    <t>BrugVeranderen, BrugWeghalen, BrugPlaatsen</t>
+    <t>BrugPlaatsen, BrugVeranderen, BrugWeghalen</t>
   </si>
   <si>
     <t>09-01-2024 13:24:05</t>
@@ -478,7 +478,7 @@
     <t>4.33</t>
   </si>
   <si>
-    <t>OntplofbareStoffenOfVoorwerpenOpslaanEtc, GasOpslaanInEenOpslagtank, GevaarlijkeStoffenOpslaanInVerpakking</t>
+    <t>GevaarlijkeStoffenOpslaanInVerpakking, GasOpslaanInEenOpslagtank, OntplofbareStoffenOfVoorwerpenOpslaanEtc</t>
   </si>
   <si>
     <t>15-01-2024 12:50:08</t>
@@ -565,13 +565,13 @@
     <t>22-02-2024 11:12:14</t>
   </si>
   <si>
-    <t>20-03-2024 15:49:34</t>
-  </si>
-  <si>
-    <t>20-03-2024 16:10:24</t>
-  </si>
-  <si>
-    <t>20-03-2024 15:49:31</t>
+    <t>20-03-2024 16:38:36</t>
+  </si>
+  <si>
+    <t>20-03-2024 16:25:46</t>
+  </si>
+  <si>
+    <t>20-03-2024 16:25:43</t>
   </si>
   <si>
     <t>steiger verwijderen</t>
@@ -631,7 +631,7 @@
     <t>4.9.2</t>
   </si>
   <si>
-    <t>BeschoeiingPlaatsen, BeschoeiingWeghalen, BeschoeiingVeranderen</t>
+    <t>BeschoeiingWeghalen, BeschoeiingVeranderen, BeschoeiingPlaatsen</t>
   </si>
   <si>
     <t>11-01-2024 10:28:29</t>
@@ -673,7 +673,7 @@
     <t>4.10.1</t>
   </si>
   <si>
-    <t>OnttrekkingsvoorzieningPlaatsen, LozingsvoorzieningPlaatsen</t>
+    <t>LozingsvoorzieningPlaatsen, OnttrekkingsvoorzieningPlaatsen</t>
   </si>
   <si>
     <t>uitstroomvoorziening of onttrekkingsvoorziening verwijderen</t>
@@ -685,7 +685,7 @@
     <t>4.10.2</t>
   </si>
   <si>
-    <t>LozingsvoorzieningPlaatsen, OnttrekkingsvoorzieningPlaatsen, LozingsvoorzieningWeghalen</t>
+    <t>OnttrekkingsvoorzieningPlaatsen, LozingsvoorzieningWeghalen, LozingsvoorzieningPlaatsen</t>
   </si>
   <si>
     <t>11-01-2024 11:36:30</t>
@@ -778,7 +778,7 @@
     <t>4.17.2</t>
   </si>
   <si>
-    <t>VerhardingWeghalen, VerhardingAanbrengen</t>
+    <t>VerhardingAanbrengen, VerhardingWeghalen</t>
   </si>
   <si>
     <t>16-01-2024 10:19:54</t>
@@ -799,7 +799,7 @@
     <t>4.14.1</t>
   </si>
   <si>
-    <t>SpeeltoestelPlaatsen, TuinmeubilairPlaatsen, AardgasBehandelen, ConstructiePlaatsen, BouwwerkInfrastructuurPlaatsen, BouwwerkAgrarischPlaatsen, ZonnepaneelPlaatsen</t>
+    <t>AardgasBehandelen, ConstructiePlaatsen, BouwwerkAgrarischPlaatsen, BouwwerkInfrastructuurPlaatsen, ZonnepaneelPlaatsen, SpeeltoestelPlaatsen, TuinmeubilairPlaatsen</t>
   </si>
   <si>
     <t>15-01-2024 10:11:25</t>
@@ -823,7 +823,7 @@
     <t>4.14.2</t>
   </si>
   <si>
-    <t>SpeeltoestelPlaatsen, SlopenVanEenBouwwwerkOfDeelDaarvanOfHetVerwijderenVanAsbest, BouwwerkAgrarischPlaatsen, ZonnepaneelPlaatsen, ConstructiePlaatsen, ConstructieWeghalen, BouwwerkInfrastructuurPlaatsen, TuinmeubilairPlaatsen</t>
+    <t>ConstructieWeghalen, SlopenVanEenBouwwwerkOfDeelDaarvanOfHetVerwijderenVanAsbest, ZonnepaneelPlaatsen, BouwwerkAgrarischPlaatsen, TuinmeubilairPlaatsen, SpeeltoestelPlaatsen, ConstructiePlaatsen, BouwwerkInfrastructuurPlaatsen</t>
   </si>
   <si>
     <t>11-01-2024 13:09:23</t>
@@ -844,7 +844,7 @@
     <t>4.16.1</t>
   </si>
   <si>
-    <t>AardgasBehandelen, AanbouwVeranderen, GebouwVeranderen, Windturbine, AanbouwPlaatsen, BouwwerkAgrarischPlaatsen, GebouwPlaatsen</t>
+    <t>AanbouwPlaatsen, GebouwVeranderen, GebouwPlaatsen, AanbouwVeranderen, BouwwerkAgrarischPlaatsen, AardgasBehandelen, Windturbine</t>
   </si>
   <si>
     <t>22-01-2024 11:55:19</t>
@@ -868,7 +868,7 @@
     <t>4.16.2</t>
   </si>
   <si>
-    <t>SlopenVanEenBouwwwerkOfDeelDaarvanOfHetVerwijderenVanAsbest, BouwwerkAgrarischPlaatsen, Windturbine, AanbouwPlaatsen</t>
+    <t>AanbouwPlaatsen, SlopenVanEenBouwwwerkOfDeelDaarvanOfHetVerwijderenVanAsbest, Windturbine, BouwwerkAgrarischPlaatsen</t>
   </si>
   <si>
     <t>11-01-2024 10:23:05</t>
@@ -925,7 +925,7 @@
     <t>4.21</t>
   </si>
   <si>
-    <t>BoomWeghalen, BoomPlanten</t>
+    <t>BoomPlanten, BoomWeghalen</t>
   </si>
   <si>
     <t>15-01-2024 14:14:21</t>
@@ -1042,7 +1042,7 @@
     <t>4.29.3</t>
   </si>
   <si>
-    <t>PeilscheidingVerwijderen, PeilscheidingAanleggen</t>
+    <t>PeilscheidingAanleggen, PeilscheidingVerwijderen</t>
   </si>
   <si>
     <t>22-01-2024 12:02:44</t>
@@ -1084,7 +1084,7 @@
     <t>4.28.2</t>
   </si>
   <si>
-    <t>CivielKunstwerkWeghalen, CivielKunstwerkPlaatsen</t>
+    <t>CivielKunstwerkPlaatsen, CivielKunstwerkWeghalen</t>
   </si>
   <si>
     <t>11-01-2024 14:16:00</t>
@@ -1144,292 +1144,292 @@
     <t>4.30.2</t>
   </si>
   <si>
+    <t>DamPlaatsen, DamWeghalen</t>
+  </si>
+  <si>
+    <t>15-01-2024 09:42:07</t>
+  </si>
+  <si>
+    <t>15-01-2024 09:42:40</t>
+  </si>
+  <si>
+    <t>15-01-2024 09:42:21</t>
+  </si>
+  <si>
+    <t>15-01-2024 09:42:30</t>
+  </si>
+  <si>
+    <t>afsluitbare duiker vervangen</t>
+  </si>
+  <si>
+    <t>nl.imow-ws0636.activiteit.AfsluitbareDuikerVerT5</t>
+  </si>
+  <si>
+    <t>4.30.3</t>
+  </si>
+  <si>
+    <t>15-01-2024 09:36:31</t>
+  </si>
+  <si>
+    <t>15-01-2024 09:38:01</t>
+  </si>
+  <si>
+    <t>15-01-2024 09:36:43</t>
+  </si>
+  <si>
+    <t>stuw aanleggen</t>
+  </si>
+  <si>
+    <t>nl.imow-ws0636.activiteit.StuwAanleggenT5</t>
+  </si>
+  <si>
+    <t>4.27.1</t>
+  </si>
+  <si>
+    <t>StuwPlaatsen</t>
+  </si>
+  <si>
+    <t>16-01-2024 13:18:22</t>
+  </si>
+  <si>
+    <t>16-01-2024 13:18:39</t>
+  </si>
+  <si>
+    <t>16-01-2024 13:18:32</t>
+  </si>
+  <si>
+    <t>stuw verwijderen</t>
+  </si>
+  <si>
+    <t>nl.imow-ws0636.activiteit.StuwVerwijderenT5</t>
+  </si>
+  <si>
+    <t>4.27.2</t>
+  </si>
+  <si>
+    <t>11-01-2024 12:21:46</t>
+  </si>
+  <si>
+    <t>11-01-2024 12:22:14</t>
+  </si>
+  <si>
+    <t>11-01-2024 12:22:05</t>
+  </si>
+  <si>
+    <t>11-01-2024 12:21:57</t>
+  </si>
+  <si>
+    <t>stuw vervangen</t>
+  </si>
+  <si>
+    <t>nl.imow-ws0636.activiteit.StuwVervangenT5</t>
+  </si>
+  <si>
+    <t>4.27.3</t>
+  </si>
+  <si>
+    <t>16-01-2024 13:37:18</t>
+  </si>
+  <si>
+    <t>16-01-2024 13:37:28</t>
+  </si>
+  <si>
+    <t>16-01-2024 13:37:32</t>
+  </si>
+  <si>
+    <t>kabel of leiding aanleggen</t>
+  </si>
+  <si>
+    <t>nl.imow-ws0636.activiteit.KabelLeidingAanleggenT5</t>
+  </si>
+  <si>
+    <t>4.11.1</t>
+  </si>
+  <si>
+    <t>KabelPlaatsen</t>
+  </si>
+  <si>
+    <t>11-01-2024 13:56:49</t>
+  </si>
+  <si>
+    <t>22-01-2024 17:23:26</t>
+  </si>
+  <si>
+    <t>22-01-2024 17:23:23</t>
+  </si>
+  <si>
+    <t>22-01-2024 17:23:30</t>
+  </si>
+  <si>
+    <t>kabel of leiding verwijderen</t>
+  </si>
+  <si>
+    <t>nl.imow-ws0636.activiteit.KabelLeidingVerwijderenT5</t>
+  </si>
+  <si>
+    <t>4.11.2</t>
+  </si>
+  <si>
+    <t>KabelPlaatsen, KabelWeghalen</t>
+  </si>
+  <si>
+    <t>11-01-2024 10:07:59</t>
+  </si>
+  <si>
+    <t>17-01-2024 13:34:45</t>
+  </si>
+  <si>
+    <t>17-01-2024 13:34:33</t>
+  </si>
+  <si>
+    <t>17-01-2024 13:34:38</t>
+  </si>
+  <si>
+    <t>bodemenergiesysteem aanleggen</t>
+  </si>
+  <si>
+    <t>nl.imow-ws0636.activiteit.BodemEnergieAanlegT5</t>
+  </si>
+  <si>
+    <t>4.23.1</t>
+  </si>
+  <si>
+    <t>BodemenergiesysteemAanleggenEnGebruiken</t>
+  </si>
+  <si>
+    <t>11-01-2024 16:36:29</t>
+  </si>
+  <si>
+    <t>11-01-2024 16:36:46</t>
+  </si>
+  <si>
+    <t>11-01-2024 16:36:58</t>
+  </si>
+  <si>
+    <t>bodemenergiesysteem verwijderen</t>
+  </si>
+  <si>
+    <t>nl.imow-ws0636.activiteit.BodemEnergieVerwijderenT5</t>
+  </si>
+  <si>
+    <t>4.23.2</t>
+  </si>
+  <si>
+    <t>15-01-2024 09:57:53</t>
+  </si>
+  <si>
+    <t>15-01-2024 09:59:05</t>
+  </si>
+  <si>
+    <t>15-01-2024 09:59:00</t>
+  </si>
+  <si>
+    <t>grondboring of sondering uitvoeren</t>
+  </si>
+  <si>
+    <t>nl.imow-ws0636.activiteit.GrondboringOfSonderingT5</t>
+  </si>
+  <si>
+    <t>4.22</t>
+  </si>
+  <si>
+    <t>GrondboringOfSonderingUitvoeren</t>
+  </si>
+  <si>
+    <t>11-01-2024 12:13:19</t>
+  </si>
+  <si>
+    <t>11-01-2024 12:13:27</t>
+  </si>
+  <si>
+    <t>11-01-2024 12:13:42</t>
+  </si>
+  <si>
+    <t>gemaal aanleggen</t>
+  </si>
+  <si>
+    <t>nl.imow-ws0636.activiteit.GemaalAanleggenT5</t>
+  </si>
+  <si>
+    <t>4.26.1</t>
+  </si>
+  <si>
+    <t>11-01-2024 10:51:25</t>
+  </si>
+  <si>
+    <t>11-01-2024 10:51:41</t>
+  </si>
+  <si>
+    <t>11-01-2024 10:51:49</t>
+  </si>
+  <si>
+    <t>gemaal verwijderen</t>
+  </si>
+  <si>
+    <t>nl.imow-ws0636.activiteit.GemaalVerwijderenT5</t>
+  </si>
+  <si>
+    <t>4.26.2</t>
+  </si>
+  <si>
+    <t>15-01-2024 13:41:36</t>
+  </si>
+  <si>
+    <t>15-01-2024 13:41:52</t>
+  </si>
+  <si>
+    <t>15-01-2024 13:41:45</t>
+  </si>
+  <si>
+    <t>15-01-2024 13:41:48</t>
+  </si>
+  <si>
+    <t>gemaal vervangen</t>
+  </si>
+  <si>
+    <t>nl.imow-ws0636.activiteit.GemaalVervangenT5</t>
+  </si>
+  <si>
+    <t>4.26.3</t>
+  </si>
+  <si>
+    <t>15-01-2024 13:24:05</t>
+  </si>
+  <si>
+    <t>15-01-2024 13:24:13</t>
+  </si>
+  <si>
+    <t>dam met duiker aanleggen</t>
+  </si>
+  <si>
+    <t>nl.imow-ws0636.activiteit.DamMetDuikerAanleggenT5</t>
+  </si>
+  <si>
+    <t>4.5.1</t>
+  </si>
+  <si>
+    <t>15-01-2024 10:51:45</t>
+  </si>
+  <si>
+    <t>15-01-2024 10:51:58</t>
+  </si>
+  <si>
+    <t>15-01-2024 10:51:55</t>
+  </si>
+  <si>
+    <t>15-01-2024 10:52:01</t>
+  </si>
+  <si>
+    <t>dam met duiker verwijderen</t>
+  </si>
+  <si>
+    <t>nl.imow-ws0636.activiteit.DamMetDuikerVerwijderenT5</t>
+  </si>
+  <si>
+    <t>4.5.2</t>
+  </si>
+  <si>
     <t>DamWeghalen, DamPlaatsen</t>
-  </si>
-  <si>
-    <t>15-01-2024 09:42:07</t>
-  </si>
-  <si>
-    <t>15-01-2024 09:42:40</t>
-  </si>
-  <si>
-    <t>15-01-2024 09:42:21</t>
-  </si>
-  <si>
-    <t>15-01-2024 09:42:30</t>
-  </si>
-  <si>
-    <t>afsluitbare duiker vervangen</t>
-  </si>
-  <si>
-    <t>nl.imow-ws0636.activiteit.AfsluitbareDuikerVerT5</t>
-  </si>
-  <si>
-    <t>4.30.3</t>
-  </si>
-  <si>
-    <t>15-01-2024 09:36:31</t>
-  </si>
-  <si>
-    <t>15-01-2024 09:38:01</t>
-  </si>
-  <si>
-    <t>15-01-2024 09:36:43</t>
-  </si>
-  <si>
-    <t>stuw aanleggen</t>
-  </si>
-  <si>
-    <t>nl.imow-ws0636.activiteit.StuwAanleggenT5</t>
-  </si>
-  <si>
-    <t>4.27.1</t>
-  </si>
-  <si>
-    <t>StuwPlaatsen</t>
-  </si>
-  <si>
-    <t>16-01-2024 13:18:22</t>
-  </si>
-  <si>
-    <t>16-01-2024 13:18:39</t>
-  </si>
-  <si>
-    <t>16-01-2024 13:18:32</t>
-  </si>
-  <si>
-    <t>stuw verwijderen</t>
-  </si>
-  <si>
-    <t>nl.imow-ws0636.activiteit.StuwVerwijderenT5</t>
-  </si>
-  <si>
-    <t>4.27.2</t>
-  </si>
-  <si>
-    <t>11-01-2024 12:21:46</t>
-  </si>
-  <si>
-    <t>11-01-2024 12:22:14</t>
-  </si>
-  <si>
-    <t>11-01-2024 12:22:05</t>
-  </si>
-  <si>
-    <t>11-01-2024 12:21:57</t>
-  </si>
-  <si>
-    <t>stuw vervangen</t>
-  </si>
-  <si>
-    <t>nl.imow-ws0636.activiteit.StuwVervangenT5</t>
-  </si>
-  <si>
-    <t>4.27.3</t>
-  </si>
-  <si>
-    <t>16-01-2024 13:37:18</t>
-  </si>
-  <si>
-    <t>16-01-2024 13:37:28</t>
-  </si>
-  <si>
-    <t>16-01-2024 13:37:32</t>
-  </si>
-  <si>
-    <t>kabel of leiding aanleggen</t>
-  </si>
-  <si>
-    <t>nl.imow-ws0636.activiteit.KabelLeidingAanleggenT5</t>
-  </si>
-  <si>
-    <t>4.11.1</t>
-  </si>
-  <si>
-    <t>KabelPlaatsen</t>
-  </si>
-  <si>
-    <t>11-01-2024 13:56:49</t>
-  </si>
-  <si>
-    <t>22-01-2024 17:23:26</t>
-  </si>
-  <si>
-    <t>22-01-2024 17:23:23</t>
-  </si>
-  <si>
-    <t>22-01-2024 17:23:30</t>
-  </si>
-  <si>
-    <t>kabel of leiding verwijderen</t>
-  </si>
-  <si>
-    <t>nl.imow-ws0636.activiteit.KabelLeidingVerwijderenT5</t>
-  </si>
-  <si>
-    <t>4.11.2</t>
-  </si>
-  <si>
-    <t>KabelWeghalen, KabelPlaatsen</t>
-  </si>
-  <si>
-    <t>11-01-2024 10:07:59</t>
-  </si>
-  <si>
-    <t>17-01-2024 13:34:45</t>
-  </si>
-  <si>
-    <t>17-01-2024 13:34:33</t>
-  </si>
-  <si>
-    <t>17-01-2024 13:34:38</t>
-  </si>
-  <si>
-    <t>bodemenergiesysteem aanleggen</t>
-  </si>
-  <si>
-    <t>nl.imow-ws0636.activiteit.BodemEnergieAanlegT5</t>
-  </si>
-  <si>
-    <t>4.23.1</t>
-  </si>
-  <si>
-    <t>BodemenergiesysteemAanleggenEnGebruiken</t>
-  </si>
-  <si>
-    <t>11-01-2024 16:36:29</t>
-  </si>
-  <si>
-    <t>11-01-2024 16:36:46</t>
-  </si>
-  <si>
-    <t>11-01-2024 16:36:58</t>
-  </si>
-  <si>
-    <t>bodemenergiesysteem verwijderen</t>
-  </si>
-  <si>
-    <t>nl.imow-ws0636.activiteit.BodemEnergieVerwijderenT5</t>
-  </si>
-  <si>
-    <t>4.23.2</t>
-  </si>
-  <si>
-    <t>15-01-2024 09:57:53</t>
-  </si>
-  <si>
-    <t>15-01-2024 09:59:05</t>
-  </si>
-  <si>
-    <t>15-01-2024 09:59:00</t>
-  </si>
-  <si>
-    <t>grondboring of sondering uitvoeren</t>
-  </si>
-  <si>
-    <t>nl.imow-ws0636.activiteit.GrondboringOfSonderingT5</t>
-  </si>
-  <si>
-    <t>4.22</t>
-  </si>
-  <si>
-    <t>GrondboringOfSonderingUitvoeren</t>
-  </si>
-  <si>
-    <t>11-01-2024 12:13:19</t>
-  </si>
-  <si>
-    <t>11-01-2024 12:13:27</t>
-  </si>
-  <si>
-    <t>11-01-2024 12:13:42</t>
-  </si>
-  <si>
-    <t>gemaal aanleggen</t>
-  </si>
-  <si>
-    <t>nl.imow-ws0636.activiteit.GemaalAanleggenT5</t>
-  </si>
-  <si>
-    <t>4.26.1</t>
-  </si>
-  <si>
-    <t>11-01-2024 10:51:25</t>
-  </si>
-  <si>
-    <t>11-01-2024 10:51:41</t>
-  </si>
-  <si>
-    <t>11-01-2024 10:51:49</t>
-  </si>
-  <si>
-    <t>gemaal verwijderen</t>
-  </si>
-  <si>
-    <t>nl.imow-ws0636.activiteit.GemaalVerwijderenT5</t>
-  </si>
-  <si>
-    <t>4.26.2</t>
-  </si>
-  <si>
-    <t>CivielKunstwerkPlaatsen, CivielKunstwerkWeghalen</t>
-  </si>
-  <si>
-    <t>15-01-2024 13:41:36</t>
-  </si>
-  <si>
-    <t>15-01-2024 13:41:52</t>
-  </si>
-  <si>
-    <t>15-01-2024 13:41:45</t>
-  </si>
-  <si>
-    <t>15-01-2024 13:41:48</t>
-  </si>
-  <si>
-    <t>gemaal vervangen</t>
-  </si>
-  <si>
-    <t>nl.imow-ws0636.activiteit.GemaalVervangenT5</t>
-  </si>
-  <si>
-    <t>4.26.3</t>
-  </si>
-  <si>
-    <t>15-01-2024 13:24:05</t>
-  </si>
-  <si>
-    <t>15-01-2024 13:24:13</t>
-  </si>
-  <si>
-    <t>dam met duiker aanleggen</t>
-  </si>
-  <si>
-    <t>nl.imow-ws0636.activiteit.DamMetDuikerAanleggenT5</t>
-  </si>
-  <si>
-    <t>4.5.1</t>
-  </si>
-  <si>
-    <t>15-01-2024 10:51:45</t>
-  </si>
-  <si>
-    <t>15-01-2024 10:51:58</t>
-  </si>
-  <si>
-    <t>15-01-2024 10:51:55</t>
-  </si>
-  <si>
-    <t>15-01-2024 10:52:01</t>
-  </si>
-  <si>
-    <t>dam met duiker verwijderen</t>
-  </si>
-  <si>
-    <t>nl.imow-ws0636.activiteit.DamMetDuikerVerwijderenT5</t>
-  </si>
-  <si>
-    <t>4.5.2</t>
   </si>
   <si>
     <t>15-01-2024 10:57:45</t>
@@ -3873,92 +3873,92 @@
         <v>451</v>
       </c>
       <c r="E68" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="F68" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="G68" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="G68" s="2" t="s">
+      <c r="H68" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="H68" s="2" t="s">
+      <c r="I68" s="2" t="s">
         <v>455</v>
-      </c>
-      <c r="I68" s="2" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="C69" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D69" s="2" t="s">
         <v>458</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>459</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>349</v>
       </c>
       <c r="F69" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="G69" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="G69" s="2" t="s">
-        <v>461</v>
-      </c>
       <c r="H69" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I69" s="2"/>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="C70" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>463</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>464</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>369</v>
       </c>
       <c r="F70" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="G70" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="G70" s="2" t="s">
+      <c r="H70" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="H70" s="2" t="s">
+      <c r="I70" s="2" t="s">
         <v>467</v>
-      </c>
-      <c r="I70" s="2" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="C71" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D71" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D71" s="2" t="s">
+      <c r="E71" s="2" t="s">
         <v>471</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>376</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>472</v>
@@ -4045,7 +4045,7 @@
         <v>492</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>376</v>
+        <v>471</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>493</v>
@@ -4101,7 +4101,7 @@
         <v>505</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>376</v>
+        <v>471</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>506</v>

</xml_diff>